<commit_message>
fixed tested points & test save location
</commit_message>
<xml_diff>
--- a/dynamics/src/dynamics/xlsx/task_point_6dof_tested_c_real.xlsx
+++ b/dynamics/src/dynamics/xlsx/task_point_6dof_tested_c_real.xlsx
@@ -30,7 +30,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -392,15 +392,15 @@
     <col min="6" max="6" style="4" width="11.862142857142858" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1">
         <v>0.04</v>
       </c>
       <c r="B1" s="1">
-        <v>-0.12</v>
+        <v>-0.13</v>
       </c>
       <c r="C1" s="1">
-        <v>-0.3</v>
+        <v>-0.34</v>
       </c>
       <c r="D1" s="2">
         <v>-31</v>
@@ -412,15 +412,15 @@
         <v>-78</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="1">
-        <v>-0.24</v>
+        <v>-0.27</v>
       </c>
       <c r="B2" s="1">
-        <v>-0.04</v>
+        <v>-0.05</v>
       </c>
       <c r="C2" s="1">
-        <v>0.27</v>
+        <v>0.3</v>
       </c>
       <c r="D2" s="2">
         <v>-104</v>
@@ -432,15 +432,15 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="1">
-        <v>0.06</v>
+        <v>0.07</v>
       </c>
       <c r="B3" s="1">
-        <v>-0.21</v>
+        <v>-0.24</v>
       </c>
       <c r="C3" s="1">
-        <v>-0.24</v>
+        <v>-0.27</v>
       </c>
       <c r="D3" s="2">
         <v>1</v>
@@ -452,15 +452,15 @@
         <v>-28</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="1">
-        <v>0.24</v>
+        <v>0.27</v>
       </c>
       <c r="B4" s="1">
-        <v>-0.1</v>
+        <v>-0.11</v>
       </c>
       <c r="C4" s="1">
-        <v>0.15</v>
+        <v>0.17</v>
       </c>
       <c r="D4" s="2">
         <v>130</v>
@@ -472,15 +472,15 @@
         <v>46</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="1">
         <v>-0.03</v>
       </c>
       <c r="B5" s="1">
-        <v>-0.1</v>
+        <v>-0.11</v>
       </c>
       <c r="C5" s="1">
-        <v>0.68</v>
+        <v>0.77</v>
       </c>
       <c r="D5" s="2">
         <v>-70</v>
@@ -492,15 +492,15 @@
         <v>60</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="1">
-        <v>0.05</v>
+        <v>0.06</v>
       </c>
       <c r="B6" s="1">
         <v>0.03</v>
       </c>
       <c r="C6" s="1">
-        <v>0.14</v>
+        <v>0.16</v>
       </c>
       <c r="D6" s="2">
         <v>-64</v>
@@ -512,15 +512,15 @@
         <v>70</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="1">
-        <v>0.15</v>
+        <v>0.17</v>
       </c>
       <c r="B7" s="1">
-        <v>-0.08</v>
+        <v>-0.09</v>
       </c>
       <c r="C7" s="1">
-        <v>-0.16</v>
+        <v>-0.18</v>
       </c>
       <c r="D7" s="2">
         <v>101</v>
@@ -532,15 +532,15 @@
         <v>-34</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="1">
-        <v>0.19</v>
+        <v>0.22</v>
       </c>
       <c r="B8" s="1">
-        <v>-0.39</v>
+        <v>-0.44</v>
       </c>
       <c r="C8" s="1">
-        <v>0.41</v>
+        <v>0.46</v>
       </c>
       <c r="D8" s="2">
         <v>69</v>
@@ -552,15 +552,15 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="1">
-        <v>-0.31</v>
+        <v>-0.35</v>
       </c>
       <c r="B9" s="1">
-        <v>-0.3</v>
+        <v>-0.33</v>
       </c>
       <c r="C9" s="1">
-        <v>0.35</v>
+        <v>0.39</v>
       </c>
       <c r="D9" s="2">
         <v>90</v>
@@ -572,15 +572,15 @@
         <v>-74</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
       <c r="A10" s="1">
-        <v>0.07</v>
+        <v>0.08</v>
       </c>
       <c r="B10" s="1">
-        <v>-0.02</v>
+        <v>-0.03</v>
       </c>
       <c r="C10" s="1">
-        <v>0.25</v>
+        <v>0.29</v>
       </c>
       <c r="D10" s="2">
         <v>-94</v>

</xml_diff>